<commit_message>
Addition of Biomek robot format and modification of tests.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Normalization_planning_v3_11_0.xlsx
+++ b/backend/fms_core/static/submission_templates/Normalization_planning_v3_11_0.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">Sample and Library Normalization Planning Template</t>
   </si>
@@ -92,7 +92,10 @@
     <t xml:space="preserve">384-well plate</t>
   </si>
   <si>
-    <t xml:space="preserve">Sample</t>
+    <t xml:space="preserve">Sample Biomek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample Janus</t>
   </si>
 </sst>
 </file>
@@ -103,7 +106,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -141,6 +144,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -218,7 +227,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -248,6 +257,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3737,7 +3750,7 @@
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A4:A555" type="list">
-      <formula1>Index!$B$2:$B$3</formula1>
+      <formula1>Index!$B$2:$B$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -3801,7 +3814,9 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
+      <c r="B4" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
     </row>

</xml_diff>